<commit_message>
Use labour min data for total autonomous and monotributista indepndent workers
</commit_message>
<xml_diff>
--- a/LIAM2_commented_code/Historical_indexes/Computed_proportions_of_monotributistas_and_autonomous_workers/Aportantes autonomos - monotributistas- asalariados por mes V2.xlsx
+++ b/LIAM2_commented_code/Historical_indexes/Computed_proportions_of_monotributistas_and_autonomous_workers/Aportantes autonomos - monotributistas- asalariados por mes V2.xlsx
@@ -1733,15 +1733,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>132</xdr:col>
-      <xdr:colOff>303480</xdr:colOff>
+      <xdr:colOff>330480</xdr:colOff>
       <xdr:row>96</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>132</xdr:col>
-      <xdr:colOff>605880</xdr:colOff>
+      <xdr:colOff>632520</xdr:colOff>
       <xdr:row>96</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>142560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1750,8 +1750,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="138090600" y="17883360"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="146358000" y="17874360"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1807,15 +1807,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>132</xdr:col>
-      <xdr:colOff>303480</xdr:colOff>
+      <xdr:colOff>330480</xdr:colOff>
       <xdr:row>96</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>132</xdr:col>
-      <xdr:colOff>605880</xdr:colOff>
+      <xdr:colOff>632520</xdr:colOff>
       <xdr:row>96</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>142560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1824,8 +1824,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="138090600" y="17883360"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="146358000" y="17874360"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1881,15 +1881,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>139</xdr:col>
-      <xdr:colOff>305640</xdr:colOff>
+      <xdr:colOff>332640</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>139</xdr:col>
-      <xdr:colOff>608040</xdr:colOff>
+      <xdr:colOff>634680</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1898,8 +1898,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="144575640" y="6033600"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="153223920" y="6024600"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1955,15 +1955,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>139</xdr:col>
-      <xdr:colOff>305640</xdr:colOff>
+      <xdr:colOff>332640</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>139</xdr:col>
-      <xdr:colOff>608040</xdr:colOff>
+      <xdr:colOff>634680</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1972,8 +1972,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="144575640" y="6033600"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="153223920" y="6024600"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2029,15 +2029,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>138</xdr:col>
-      <xdr:colOff>279000</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:colOff>306000</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>145</xdr:col>
-      <xdr:colOff>538200</xdr:colOff>
+      <xdr:colOff>564840</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2051,8 +2051,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="143410320" y="14162400"/>
-          <a:ext cx="8229240" cy="3378240"/>
+          <a:off x="151992000" y="14153400"/>
+          <a:ext cx="8695440" cy="3377880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2067,15 +2067,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>169</xdr:col>
-      <xdr:colOff>303480</xdr:colOff>
+      <xdr:colOff>330480</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>169</xdr:col>
-      <xdr:colOff>605880</xdr:colOff>
+      <xdr:colOff>632520</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2084,8 +2084,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="170610840" y="6033600"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="180785160" y="6024600"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2141,15 +2141,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>169</xdr:col>
-      <xdr:colOff>303480</xdr:colOff>
+      <xdr:colOff>330480</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>169</xdr:col>
-      <xdr:colOff>605880</xdr:colOff>
+      <xdr:colOff>632520</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2158,8 +2158,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="170610840" y="6033600"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="180785160" y="6024600"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2215,15 +2215,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>193</xdr:col>
-      <xdr:colOff>304200</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>193</xdr:col>
-      <xdr:colOff>606600</xdr:colOff>
+      <xdr:colOff>633240</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2232,8 +2232,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="196205400" y="6033600"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="207850320" y="6024600"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2289,15 +2289,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>193</xdr:col>
-      <xdr:colOff>304200</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>193</xdr:col>
-      <xdr:colOff>606600</xdr:colOff>
+      <xdr:colOff>633240</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2306,8 +2306,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="196205400" y="6033600"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="207850320" y="6024600"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2363,15 +2363,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>174</xdr:col>
-      <xdr:colOff>305280</xdr:colOff>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>174</xdr:col>
-      <xdr:colOff>607680</xdr:colOff>
+      <xdr:colOff>634320</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2380,8 +2380,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="175714920" y="6033600"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="186178680" y="6024600"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2437,15 +2437,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>174</xdr:col>
-      <xdr:colOff>305280</xdr:colOff>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>174</xdr:col>
-      <xdr:colOff>607680</xdr:colOff>
+      <xdr:colOff>634320</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2454,8 +2454,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="175714920" y="6033600"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="186178680" y="6024600"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2511,15 +2511,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>217</xdr:col>
-      <xdr:colOff>305280</xdr:colOff>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>217</xdr:col>
-      <xdr:colOff>607680</xdr:colOff>
+      <xdr:colOff>634320</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2528,8 +2528,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="220994280" y="6080400"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="234111960" y="6071400"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2585,15 +2585,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>217</xdr:col>
-      <xdr:colOff>305280</xdr:colOff>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>217</xdr:col>
-      <xdr:colOff>607680</xdr:colOff>
+      <xdr:colOff>634320</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2602,8 +2602,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="220994280" y="6080400"/>
-          <a:ext cx="302400" cy="360"/>
+          <a:off x="234111960" y="6071400"/>
+          <a:ext cx="302040" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2659,15 +2659,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>241</xdr:col>
-      <xdr:colOff>571680</xdr:colOff>
+      <xdr:colOff>598680</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>242</xdr:col>
-      <xdr:colOff>200520</xdr:colOff>
+      <xdr:colOff>227160</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>147960</xdr:rowOff>
+      <xdr:rowOff>138960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2676,8 +2676,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="245157120" y="6080760"/>
-          <a:ext cx="700560" cy="360"/>
+          <a:off x="259638480" y="6071760"/>
+          <a:ext cx="762120" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2733,15 +2733,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>241</xdr:col>
-      <xdr:colOff>571680</xdr:colOff>
+      <xdr:colOff>598680</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>242</xdr:col>
-      <xdr:colOff>200520</xdr:colOff>
+      <xdr:colOff>227160</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>147960</xdr:rowOff>
+      <xdr:rowOff>138960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2750,8 +2750,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="245157120" y="6080760"/>
-          <a:ext cx="700560" cy="360"/>
+          <a:off x="259638480" y="6071760"/>
+          <a:ext cx="762120" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2814,64 +2814,64 @@
   </sheetPr>
   <dimension ref="A1:JA315"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CO1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="AA5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="CO1" activeCellId="0" sqref="CO1"/>
-      <selection pane="bottomLeft" activeCell="CT16" activeCellId="0" sqref="CT16:CT17"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="134" min="34" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="135" min="135" style="0" width="12.75"/>
-    <col collapsed="false" hidden="false" max="137" min="136" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="148" min="138" style="0" width="16.1377551020408"/>
-    <col collapsed="false" hidden="false" max="160" min="149" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="172" min="161" style="0" width="13.1683673469388"/>
-    <col collapsed="false" hidden="false" max="184" min="173" style="0" width="16.4081632653061"/>
-    <col collapsed="false" hidden="false" max="196" min="185" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="208" min="197" style="0" width="14.7755102040816"/>
-    <col collapsed="false" hidden="false" max="220" min="209" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="232" min="221" style="0" width="13.1683673469388"/>
-    <col collapsed="false" hidden="false" max="244" min="233" style="0" width="15.1887755102041"/>
-    <col collapsed="false" hidden="false" max="249" min="245" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="250" min="250" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="251" min="251" style="0" width="20.9234693877551"/>
-    <col collapsed="false" hidden="false" max="254" min="252" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="255" min="255" style="0" width="17.0816326530612"/>
-    <col collapsed="false" hidden="false" max="256" min="256" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="257" min="257" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="15.7244897959184"/>
-    <col collapsed="false" hidden="false" max="259" min="259" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="13.969387755102"/>
-    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="262" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.9030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.1887755102041"/>
+    <col collapsed="false" hidden="false" max="134" min="34" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="135" min="135" style="0" width="13.4336734693878"/>
+    <col collapsed="false" hidden="false" max="137" min="136" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="148" min="138" style="0" width="17.0816326530612"/>
+    <col collapsed="false" hidden="false" max="160" min="149" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="172" min="161" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="184" min="173" style="0" width="17.3520408163265"/>
+    <col collapsed="false" hidden="false" max="196" min="185" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="208" min="197" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="220" min="209" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="232" min="221" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="244" min="233" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="249" min="245" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="250" min="250" style="0" width="20.4489795918367"/>
+    <col collapsed="false" hidden="false" max="251" min="251" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="254" min="252" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="255" min="255" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="256" min="256" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="257" min="257" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="16.6734693877551"/>
+    <col collapsed="false" hidden="false" max="259" min="259" style="0" width="16.2602040816327"/>
+    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="14.7755102040816"/>
+    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="13.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="262" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -69498,12 +69498,12 @@
   <dimension ref="A1:IS39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N38" activeCellId="1" sqref="CT16:CT17 N38"/>
+      <selection pane="topLeft" activeCell="N38" activeCellId="0" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" s="155" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>